<commit_message>
second phase for about us.....
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/server_page.xlsx
+++ b/apps/features/backlog/android/server_page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\apps\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F5B3BF-CAAC-43C5-9243-F6AEA735703D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F14D70-800B-439F-9390-6E4A06B760BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -51,9 +51,6 @@
   <si>
     <t>1. VPN app installed and launched.
 2. User logged in.</t>
-  </si>
-  <si>
-    <t>Verify that the user can select a preferred server for the VPN connection.</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
@@ -117,9 +114,6 @@
 3.The user is on the server selection screen</t>
   </si>
   <si>
-    <t>Verify that the VPN app successfully disconnects to a gaming server.</t>
-  </si>
-  <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
 2. Open the installed SymlexVPN Application.
 3. Login with proper credentials
@@ -137,9 +131,6 @@
     <t>1. VPN app installed and launched.
 2. User logged in.
 3. The device has a stable internet connection.</t>
-  </si>
-  <si>
-    <t>Verify that the VPN app successfully connects to a server.</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the mobile.
@@ -353,6 +344,18 @@
   </si>
   <si>
     <t>Scenario : Server Page</t>
+  </si>
+  <si>
+    <t>verify that the user can select a preferred server for the VPN connection.</t>
+  </si>
+  <si>
+    <t>verify that the VPN app successfully disconnects to a gaming server.</t>
+  </si>
+  <si>
+    <t>verify that the VPN app successfully connects to a server</t>
+  </si>
+  <si>
+    <t>verify that the VPN app successfully disconnects to a gaming server</t>
   </si>
 </sst>
 </file>
@@ -1343,8 +1346,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:G19"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1361,7 +1364,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1467,16 +1470,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>7</v>
@@ -1503,22 +1506,22 @@
     </row>
     <row r="5" spans="1:26" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="5"/>
@@ -1543,22 +1546,22 @@
     </row>
     <row r="6" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="5"/>
@@ -1583,22 +1586,22 @@
     </row>
     <row r="7" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>27</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
@@ -1623,22 +1626,22 @@
     </row>
     <row r="8" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="5"/>
@@ -1663,22 +1666,22 @@
     </row>
     <row r="9" spans="1:26" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>34</v>
-      </c>
       <c r="F9" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="7"/>
@@ -1703,22 +1706,22 @@
     </row>
     <row r="10" spans="1:26" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>38</v>
-      </c>
       <c r="F10" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="7"/>
@@ -1743,22 +1746,22 @@
     </row>
     <row r="11" spans="1:26" ht="114.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="F11" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="1"/>
@@ -1783,22 +1786,22 @@
     </row>
     <row r="12" spans="1:26" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="F12" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="1"/>
@@ -1823,22 +1826,22 @@
     </row>
     <row r="13" spans="1:26" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>50</v>
-      </c>
       <c r="F13" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="1"/>
@@ -1863,22 +1866,22 @@
     </row>
     <row r="14" spans="1:26" ht="154.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="E14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="F14" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="1"/>
@@ -1903,22 +1906,22 @@
     </row>
     <row r="15" spans="1:26" ht="168" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="E15" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>60</v>
-      </c>
       <c r="F15" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="1"/>
@@ -1943,22 +1946,22 @@
     </row>
     <row r="16" spans="1:26" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>65</v>
-      </c>
       <c r="F16" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="23"/>
@@ -1983,22 +1986,22 @@
     </row>
     <row r="17" spans="1:26" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>69</v>
-      </c>
       <c r="F17" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="1"/>
@@ -2023,22 +2026,22 @@
     </row>
     <row r="18" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>74</v>
-      </c>
       <c r="F18" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="1"/>

</xml_diff>

<commit_message>
add new payment gateway.... admin panel startef...
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/server_page.xlsx
+++ b/apps/features/backlog/android/server_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\apps\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F14D70-800B-439F-9390-6E4A06B760BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF1B2F4-53AC-45D2-AB65-02AF7B7344FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -356,6 +356,19 @@
   </si>
   <si>
     <t>verify that the VPN app successfully disconnects to a gaming server</t>
+  </si>
+  <si>
+    <t>test entering valid search query</t>
+  </si>
+  <si>
+    <t>TC_SYM_SP_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. go to playstore and install SymlexVPN in the mobile
+2. open the installed SymlexVPN application
+3. login with proper credentials
+4. navigate to the VPN connection page
+5. </t>
   </si>
 </sst>
 </file>
@@ -1346,8 +1359,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2047,7 @@
       <c r="C18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="13" t="s">
         <v>70</v>
       </c>
       <c r="E18" s="18" t="s">
@@ -2065,10 +2078,18 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>

</xml_diff>